<commit_message>
The loadings are saved
The loadings have been saved to an excel table which can format the data so it is easier to interpret
</commit_message>
<xml_diff>
--- a/PCA/CorrelationsMatrixTestForHighCorrelations.xlsx
+++ b/PCA/CorrelationsMatrixTestForHighCorrelations.xlsx
@@ -573,8 +573,8 @@
   </sheetPr>
   <dimension ref="A1:AO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A41"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>